<commit_message>
updating repo inline with all changes
</commit_message>
<xml_diff>
--- a/topology_linker/out/comparisons.xlsx
+++ b/topology_linker/out/comparisons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hutchinsons\Documents\MI - PROJECTS\topology_linker\topology_linker\out\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90209EF3-0FF2-4C81-9FED-C6D89607C165}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F31301-0763-4B21-A0E7-D936C2848458}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{C0AC8A49-FEB8-4CBC-944C-4C4F981CE605}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{C0AC8A49-FEB8-4CBC-944C-4C4F981CE605}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t>Pool</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>(REPORTED)</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -336,7 +339,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-AU" baseline="0"/>
-              <a:t> into pool</a:t>
+              <a:t> into pool (5% error bars)</a:t>
             </a:r>
             <a:endParaRPr lang="en-AU"/>
           </a:p>
@@ -714,20 +717,35 @@
             <c:symbol val="x"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:pattFill prst="pct5">
-                <a:fgClr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
                   <a:srgbClr val="C00000"/>
-                </a:fgClr>
-                <a:bgClr>
-                  <a:schemeClr val="bg1"/>
-                </a:bgClr>
-              </a:pattFill>
-              <a:ln w="9525">
-                <a:noFill/>
+                </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="8"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$3:$A$18</c:f>
@@ -915,7 +933,9 @@
       <c:valAx>
         <c:axId val="1297173440"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
+          <c:min val="10"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1047,6 +1067,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.89007661778387592"/>
+          <c:y val="8.1093173722633569E-2"/>
+          <c:w val="9.3495815336039137E-2"/>
+          <c:h val="0.1064262243306337"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="1"/>
       <c:spPr>
         <a:noFill/>
@@ -1154,7 +1184,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-AU" baseline="0"/>
-              <a:t> delivered</a:t>
+              <a:t> delivered (5% error bar)</a:t>
             </a:r>
             <a:endParaRPr lang="en-AU"/>
           </a:p>
@@ -1466,7 +1496,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="C00000"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1479,6 +1509,25 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$I$3:$I$18</c:f>
@@ -1609,7 +1658,10 @@
       <c:valAx>
         <c:axId val="1297173440"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
+          <c:max val="1050"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1740,10 +1792,12 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="tr"/>
       <c:overlay val="1"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -4124,7 +4178,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{E544AB0B-1222-4F8F-8A3E-E57630E95256}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="110" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="85" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4135,7 +4189,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{47804AC3-1D3C-4033-AEF1-752940A81325}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="110" workbookViewId="0" zoomToFit="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4146,7 +4200,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{12AC294D-78CB-4DD8-A734-0E22C9E67FFF}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="110" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4157,7 +4211,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9273886" cy="6052705"/>
+    <xdr:ext cx="9277089" cy="6041199"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -4190,7 +4244,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9273886" cy="6052705"/>
+    <xdr:ext cx="9277089" cy="6041199"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -4223,7 +4277,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9273886" cy="6052705"/>
+    <xdr:ext cx="9295086" cy="6054397"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -4549,10 +4603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2B84F25-E1A0-4F6D-A3D7-AD0B8234E026}">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4650,11 +4704,11 @@
         <v>-262.5</v>
       </c>
       <c r="K3">
-        <f>C3-I3</f>
-        <v>29.099999999999994</v>
+        <f>C3-F3</f>
+        <v>35.199999999999989</v>
       </c>
       <c r="L3">
-        <f>D3-J3</f>
+        <f t="shared" ref="L3:L18" si="0">D3-J3</f>
         <v>23.800000000000011</v>
       </c>
       <c r="M3" t="s">
@@ -4704,11 +4758,11 @@
         <v>390.1</v>
       </c>
       <c r="K4">
-        <f>C4-I4</f>
-        <v>14.199999999999989</v>
+        <f t="shared" ref="K4:K18" si="1">C4-F4</f>
+        <v>16</v>
       </c>
       <c r="L4">
-        <f>D4-J4</f>
+        <f t="shared" si="0"/>
         <v>-68.600000000000023</v>
       </c>
       <c r="M4" t="s">
@@ -4754,11 +4808,11 @@
         <v>168</v>
       </c>
       <c r="K5">
-        <f>C5-I5</f>
-        <v>-0.20000000000000284</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="L5">
-        <f>D5-J5</f>
+        <f t="shared" si="0"/>
         <v>-2.0999999999999943</v>
       </c>
     </row>
@@ -4794,11 +4848,11 @@
         <v>-215.7</v>
       </c>
       <c r="K6">
-        <f>C6-I6</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L6">
-        <f>D6-J6</f>
+        <f t="shared" si="0"/>
         <v>-12.400000000000006</v>
       </c>
     </row>
@@ -4836,11 +4890,11 @@
         <v>216.70000000000005</v>
       </c>
       <c r="K7">
-        <f>C7-I7</f>
-        <v>-292.5</v>
+        <f t="shared" si="1"/>
+        <v>-4.8000000000000682</v>
       </c>
       <c r="L7">
-        <f>D7-J7</f>
+        <f t="shared" si="0"/>
         <v>293.99999999999994</v>
       </c>
       <c r="M7" t="s">
@@ -4885,11 +4939,11 @@
         <v>7.5</v>
       </c>
       <c r="K8">
-        <f>C8-I8</f>
-        <v>-24.1</v>
+        <f t="shared" si="1"/>
+        <v>2.6999999999999993</v>
       </c>
       <c r="L8">
-        <f>D8-J8</f>
+        <f t="shared" si="0"/>
         <v>17.8</v>
       </c>
     </row>
@@ -4925,11 +4979,11 @@
         <v>-38.200000000000003</v>
       </c>
       <c r="K9">
-        <f>C9-I9</f>
-        <v>-0.29999999999999716</v>
+        <f t="shared" si="1"/>
+        <v>-9.9999999999994316E-2</v>
       </c>
       <c r="L9">
-        <f>D9-J9</f>
+        <f t="shared" si="0"/>
         <v>-1.0999999999999943</v>
       </c>
     </row>
@@ -4965,11 +5019,11 @@
         <v>69</v>
       </c>
       <c r="K10">
-        <f>C10-I10</f>
-        <v>-8.6999999999999318</v>
+        <f t="shared" si="1"/>
+        <v>9.8999999999999773</v>
       </c>
       <c r="L10">
-        <f>D10-J10</f>
+        <f t="shared" si="0"/>
         <v>17.700000000000003</v>
       </c>
     </row>
@@ -5005,11 +5059,11 @@
         <v>64.7</v>
       </c>
       <c r="K11">
-        <f>C11-I11</f>
-        <v>6.1000000000000085</v>
+        <f t="shared" si="1"/>
+        <v>-2.8999999999999915</v>
       </c>
       <c r="L11">
-        <f>D11-J11</f>
+        <f t="shared" si="0"/>
         <v>15.299999999999997</v>
       </c>
       <c r="M11" t="s">
@@ -5048,11 +5102,11 @@
         <v>-90.3</v>
       </c>
       <c r="K12">
-        <f>C12-I12</f>
-        <v>-18.600000000000023</v>
+        <f t="shared" si="1"/>
+        <v>-0.80000000000001137</v>
       </c>
       <c r="L12">
-        <f>D12-J12</f>
+        <f t="shared" si="0"/>
         <v>20.899999999999991</v>
       </c>
     </row>
@@ -5088,11 +5142,11 @@
         <v>73.5</v>
       </c>
       <c r="K13">
-        <f>C13-I13</f>
-        <v>-22.699999999999989</v>
+        <f t="shared" si="1"/>
+        <v>-4</v>
       </c>
       <c r="L13">
-        <f>D13-J13</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
@@ -5128,11 +5182,11 @@
         <v>-31.1</v>
       </c>
       <c r="K14">
-        <f>C14-I14</f>
-        <v>-36.900000000000006</v>
+        <f t="shared" si="1"/>
+        <v>-1.5</v>
       </c>
       <c r="L14">
-        <f>D14-J14</f>
+        <f t="shared" si="0"/>
         <v>37.700000000000003</v>
       </c>
     </row>
@@ -5168,11 +5222,11 @@
         <v>-7</v>
       </c>
       <c r="K15">
-        <f>C15-I15</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L15">
-        <f>D15-J15</f>
+        <f t="shared" si="0"/>
         <v>-0.40000000000000036</v>
       </c>
     </row>
@@ -5208,15 +5262,15 @@
         <v>33.799999999999997</v>
       </c>
       <c r="K16">
-        <f>C16-I16</f>
-        <v>2.0999999999999943</v>
+        <f t="shared" si="1"/>
+        <v>9.9999999999994316E-2</v>
       </c>
       <c r="L16">
-        <f>D16-J16</f>
+        <f t="shared" si="0"/>
         <v>0.90000000000000568</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -5248,15 +5302,15 @@
         <v>-0.3</v>
       </c>
       <c r="K17">
-        <f>C17-I17</f>
-        <v>8.5999999999999979</v>
+        <f t="shared" si="1"/>
+        <v>1.0999999999999979</v>
       </c>
       <c r="L17">
-        <f>D17-J17</f>
+        <f t="shared" si="0"/>
         <v>-2.4000000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
@@ -5288,15 +5342,15 @@
         <v>-14</v>
       </c>
       <c r="K18">
-        <f>C18-I18</f>
-        <v>5.7000000000000011</v>
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="L18">
-        <f>D18-J18</f>
+        <f t="shared" si="0"/>
         <v>10.5</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C19">
         <f>SUM(C3:C18)</f>
         <v>2858.6000000000004</v>
@@ -5309,6 +5363,254 @@
         <f>SUM(I3:I18)</f>
         <v>3196.8</v>
       </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="S22" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="str">
+        <f>B1</f>
+        <v>(INTEGRATED)</v>
+      </c>
+      <c r="C23" s="3">
+        <v>200</v>
+      </c>
+      <c r="D23" s="3">
+        <v>381.5</v>
+      </c>
+      <c r="E23" s="3">
+        <v>55.9</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>681.9</v>
+      </c>
+      <c r="H23" s="3">
+        <v>26.5</v>
+      </c>
+      <c r="I23" s="3">
+        <v>42.7</v>
+      </c>
+      <c r="J23" s="3">
+        <v>536.1</v>
+      </c>
+      <c r="K23" s="3">
+        <v>111.4</v>
+      </c>
+      <c r="L23" s="3">
+        <v>288.89999999999998</v>
+      </c>
+      <c r="M23" s="3">
+        <v>172.3</v>
+      </c>
+      <c r="N23" s="3">
+        <v>111</v>
+      </c>
+      <c r="O23" s="3">
+        <v>0</v>
+      </c>
+      <c r="P23" s="3">
+        <v>203.4</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>27.2</v>
+      </c>
+      <c r="R23" s="3">
+        <v>19.8</v>
+      </c>
+      <c r="S23" s="3">
+        <f>SUM(C23:R23)</f>
+        <v>2858.6000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="str">
+        <f>E1</f>
+        <v>(RTU)</v>
+      </c>
+      <c r="C24" s="9">
+        <v>164.8</v>
+      </c>
+      <c r="D24" s="9">
+        <v>365.5</v>
+      </c>
+      <c r="E24" s="3">
+        <v>54.9</v>
+      </c>
+      <c r="F24" s="9">
+        <v>0</v>
+      </c>
+      <c r="G24" s="9">
+        <v>686.7</v>
+      </c>
+      <c r="H24" s="9">
+        <v>23.8</v>
+      </c>
+      <c r="I24" s="9">
+        <v>42.8</v>
+      </c>
+      <c r="J24" s="9">
+        <v>526.20000000000005</v>
+      </c>
+      <c r="K24" s="9">
+        <v>114.3</v>
+      </c>
+      <c r="L24" s="9">
+        <v>289.7</v>
+      </c>
+      <c r="M24" s="9">
+        <v>176.3</v>
+      </c>
+      <c r="N24" s="9">
+        <v>112.5</v>
+      </c>
+      <c r="O24" s="9">
+        <v>0</v>
+      </c>
+      <c r="P24" s="9">
+        <v>203.3</v>
+      </c>
+      <c r="Q24" s="9">
+        <v>26.1</v>
+      </c>
+      <c r="R24" s="3">
+        <v>19.3</v>
+      </c>
+      <c r="S24" s="3">
+        <f t="shared" ref="S24:S25" si="2">SUM(C24:R24)</f>
+        <v>2806.2000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="str">
+        <f>H1</f>
+        <v>(REPORTED)</v>
+      </c>
+      <c r="C25" s="3">
+        <v>170.9</v>
+      </c>
+      <c r="D25" s="3">
+        <v>367.3</v>
+      </c>
+      <c r="E25" s="3">
+        <v>56.1</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3">
+        <v>974.4</v>
+      </c>
+      <c r="H25" s="3">
+        <v>50.6</v>
+      </c>
+      <c r="I25" s="3">
+        <v>43</v>
+      </c>
+      <c r="J25" s="3">
+        <v>544.79999999999995</v>
+      </c>
+      <c r="K25" s="3">
+        <v>105.3</v>
+      </c>
+      <c r="L25" s="3">
+        <v>307.5</v>
+      </c>
+      <c r="M25" s="3">
+        <v>195</v>
+      </c>
+      <c r="N25" s="3">
+        <v>147.9</v>
+      </c>
+      <c r="O25" s="3">
+        <v>0</v>
+      </c>
+      <c r="P25" s="3">
+        <v>201.3</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="R25" s="3">
+        <v>14.1</v>
+      </c>
+      <c r="S25" s="3">
+        <f t="shared" si="2"/>
+        <v>3196.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K3:K18">

</xml_diff>